<commit_message>
Update PRIM model with UGA functional version
</commit_message>
<xml_diff>
--- a/src/workflow/4_PRIM/prim_files_creator_cntrl.xlsx
+++ b/src/workflow/4_PRIM/prim_files_creator_cntrl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\AFR_RDM\src\workflow\4_PRIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9990EDCB-A909-4F34-9C24-32EC29A2BD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199EB5C5-944C-4244-B26E-5FD81BB9180B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="match_exp_ana" sheetId="5" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="120">
   <si>
     <t>YES</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>AnnualTechnologyEmission</t>
+  </si>
+  <si>
+    <t>AccumulatedAnnualDemand</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60477372-007B-42DB-8434-89BB151CD17B}">
-  <dimension ref="A1:C163"/>
+  <dimension ref="A1:C164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1932,7 @@
         <v>110</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>17</v>
@@ -1940,7 +1943,7 @@
         <v>110</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>17</v>
@@ -1951,7 +1954,7 @@
         <v>110</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>17</v>
@@ -1962,7 +1965,7 @@
         <v>110</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>17</v>
@@ -1973,7 +1976,7 @@
         <v>110</v>
       </c>
       <c r="B75" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>17</v>
@@ -1984,7 +1987,7 @@
         <v>110</v>
       </c>
       <c r="B76" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>17</v>
@@ -1995,7 +1998,7 @@
         <v>110</v>
       </c>
       <c r="B77" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>17</v>
@@ -2006,7 +2009,7 @@
         <v>110</v>
       </c>
       <c r="B78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>17</v>
@@ -2017,7 +2020,7 @@
         <v>110</v>
       </c>
       <c r="B79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>17</v>
@@ -2028,7 +2031,7 @@
         <v>110</v>
       </c>
       <c r="B80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>17</v>
@@ -2039,7 +2042,7 @@
         <v>110</v>
       </c>
       <c r="B81" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>17</v>
@@ -2050,7 +2053,7 @@
         <v>110</v>
       </c>
       <c r="B82" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>17</v>
@@ -2061,7 +2064,7 @@
         <v>110</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>17</v>
@@ -2072,43 +2075,43 @@
         <v>110</v>
       </c>
       <c r="B84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B86" t="s">
         <v>33</v>
       </c>
-      <c r="C85" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="C86" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B87" t="s">
-        <v>11</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2116,10 +2119,10 @@
         <v>111</v>
       </c>
       <c r="B88" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2127,7 +2130,7 @@
         <v>111</v>
       </c>
       <c r="B89" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>15</v>
@@ -2138,7 +2141,7 @@
         <v>111</v>
       </c>
       <c r="B90" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>15</v>
@@ -2149,10 +2152,10 @@
         <v>111</v>
       </c>
       <c r="B91" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2160,7 +2163,7 @@
         <v>111</v>
       </c>
       <c r="B92" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>17</v>
@@ -2171,7 +2174,7 @@
         <v>111</v>
       </c>
       <c r="B93" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>17</v>
@@ -2182,7 +2185,7 @@
         <v>111</v>
       </c>
       <c r="B94" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>17</v>
@@ -2193,7 +2196,7 @@
         <v>111</v>
       </c>
       <c r="B95" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>17</v>
@@ -2204,7 +2207,7 @@
         <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>17</v>
@@ -2215,7 +2218,7 @@
         <v>111</v>
       </c>
       <c r="B97" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>17</v>
@@ -2226,43 +2229,43 @@
         <v>111</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B99" t="s">
+        <v>40</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B100" t="s">
         <v>118</v>
       </c>
-      <c r="C99" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B100" s="4" t="s">
+      <c r="C100" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C101" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B101" t="s">
-        <v>11</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2270,10 +2273,10 @@
         <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2281,7 +2284,7 @@
         <v>106</v>
       </c>
       <c r="B103" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>15</v>
@@ -2292,7 +2295,7 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>15</v>
@@ -2303,10 +2306,10 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2314,10 +2317,10 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2325,10 +2328,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2336,7 +2339,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>15</v>
@@ -2347,7 +2350,7 @@
         <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>15</v>
@@ -2358,7 +2361,7 @@
         <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>15</v>
@@ -2369,10 +2372,10 @@
         <v>106</v>
       </c>
       <c r="B111" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2380,7 +2383,7 @@
         <v>106</v>
       </c>
       <c r="B112" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>17</v>
@@ -2391,7 +2394,7 @@
         <v>106</v>
       </c>
       <c r="B113" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>17</v>
@@ -2402,7 +2405,7 @@
         <v>106</v>
       </c>
       <c r="B114" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>17</v>
@@ -2413,7 +2416,7 @@
         <v>106</v>
       </c>
       <c r="B115" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>17</v>
@@ -2424,7 +2427,7 @@
         <v>106</v>
       </c>
       <c r="B116" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>17</v>
@@ -2435,7 +2438,7 @@
         <v>106</v>
       </c>
       <c r="B117" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>17</v>
@@ -2446,7 +2449,7 @@
         <v>106</v>
       </c>
       <c r="B118" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>17</v>
@@ -2457,7 +2460,7 @@
         <v>106</v>
       </c>
       <c r="B119" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>17</v>
@@ -2468,7 +2471,7 @@
         <v>106</v>
       </c>
       <c r="B120" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>17</v>
@@ -2479,7 +2482,7 @@
         <v>106</v>
       </c>
       <c r="B121" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>17</v>
@@ -2490,7 +2493,7 @@
         <v>106</v>
       </c>
       <c r="B122" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>17</v>
@@ -2501,7 +2504,7 @@
         <v>106</v>
       </c>
       <c r="B123" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>17</v>
@@ -2512,7 +2515,7 @@
         <v>106</v>
       </c>
       <c r="B124" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>17</v>
@@ -2523,7 +2526,7 @@
         <v>106</v>
       </c>
       <c r="B125" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>17</v>
@@ -2534,7 +2537,7 @@
         <v>106</v>
       </c>
       <c r="B126" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>17</v>
@@ -2545,7 +2548,7 @@
         <v>106</v>
       </c>
       <c r="B127" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>17</v>
@@ -2556,7 +2559,7 @@
         <v>106</v>
       </c>
       <c r="B128" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>17</v>
@@ -2567,7 +2570,7 @@
         <v>106</v>
       </c>
       <c r="B129" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C129" s="7" t="s">
         <v>17</v>
@@ -2578,7 +2581,7 @@
         <v>106</v>
       </c>
       <c r="B130" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C130" s="7" t="s">
         <v>17</v>
@@ -2589,7 +2592,7 @@
         <v>106</v>
       </c>
       <c r="B131" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C131" s="7" t="s">
         <v>17</v>
@@ -2600,7 +2603,7 @@
         <v>106</v>
       </c>
       <c r="B132" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C132" s="7" t="s">
         <v>17</v>
@@ -2611,7 +2614,7 @@
         <v>106</v>
       </c>
       <c r="B133" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>17</v>
@@ -2622,7 +2625,7 @@
         <v>106</v>
       </c>
       <c r="B134" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C134" s="7" t="s">
         <v>17</v>
@@ -2633,7 +2636,7 @@
         <v>106</v>
       </c>
       <c r="B135" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>17</v>
@@ -2644,7 +2647,7 @@
         <v>106</v>
       </c>
       <c r="B136" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C136" s="7" t="s">
         <v>17</v>
@@ -2655,7 +2658,7 @@
         <v>106</v>
       </c>
       <c r="B137" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>17</v>
@@ -2666,7 +2669,7 @@
         <v>106</v>
       </c>
       <c r="B138" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C138" s="7" t="s">
         <v>17</v>
@@ -2677,7 +2680,7 @@
         <v>106</v>
       </c>
       <c r="B139" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C139" s="7" t="s">
         <v>17</v>
@@ -2688,7 +2691,7 @@
         <v>106</v>
       </c>
       <c r="B140" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C140" s="7" t="s">
         <v>17</v>
@@ -2699,7 +2702,7 @@
         <v>106</v>
       </c>
       <c r="B141" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C141" s="7" t="s">
         <v>17</v>
@@ -2710,7 +2713,7 @@
         <v>106</v>
       </c>
       <c r="B142" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C142" s="7" t="s">
         <v>17</v>
@@ -2721,7 +2724,7 @@
         <v>106</v>
       </c>
       <c r="B143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C143" s="7" t="s">
         <v>17</v>
@@ -2732,7 +2735,7 @@
         <v>106</v>
       </c>
       <c r="B144" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C144" s="7" t="s">
         <v>17</v>
@@ -2743,7 +2746,7 @@
         <v>106</v>
       </c>
       <c r="B145" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C145" s="7" t="s">
         <v>17</v>
@@ -2754,7 +2757,7 @@
         <v>106</v>
       </c>
       <c r="B146" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C146" s="7" t="s">
         <v>17</v>
@@ -2765,7 +2768,7 @@
         <v>106</v>
       </c>
       <c r="B147" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>17</v>
@@ -2776,7 +2779,7 @@
         <v>106</v>
       </c>
       <c r="B148" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C148" s="7" t="s">
         <v>17</v>
@@ -2787,7 +2790,7 @@
         <v>106</v>
       </c>
       <c r="B149" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C149" s="7" t="s">
         <v>17</v>
@@ -2798,7 +2801,7 @@
         <v>106</v>
       </c>
       <c r="B150" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C150" s="7" t="s">
         <v>17</v>
@@ -2809,7 +2812,7 @@
         <v>106</v>
       </c>
       <c r="B151" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>17</v>
@@ -2820,7 +2823,7 @@
         <v>106</v>
       </c>
       <c r="B152" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>17</v>
@@ -2831,7 +2834,7 @@
         <v>106</v>
       </c>
       <c r="B153" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>17</v>
@@ -2842,7 +2845,7 @@
         <v>106</v>
       </c>
       <c r="B154" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C154" s="7" t="s">
         <v>17</v>
@@ -2853,7 +2856,7 @@
         <v>106</v>
       </c>
       <c r="B155" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C155" s="7" t="s">
         <v>17</v>
@@ -2864,7 +2867,7 @@
         <v>106</v>
       </c>
       <c r="B156" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C156" s="7" t="s">
         <v>17</v>
@@ -2875,7 +2878,7 @@
         <v>106</v>
       </c>
       <c r="B157" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>17</v>
@@ -2886,7 +2889,7 @@
         <v>106</v>
       </c>
       <c r="B158" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>17</v>
@@ -2897,7 +2900,7 @@
         <v>106</v>
       </c>
       <c r="B159" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>17</v>
@@ -2908,7 +2911,7 @@
         <v>106</v>
       </c>
       <c r="B160" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C160" s="7" t="s">
         <v>17</v>
@@ -2919,7 +2922,7 @@
         <v>106</v>
       </c>
       <c r="B161" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>17</v>
@@ -2930,20 +2933,31 @@
         <v>106</v>
       </c>
       <c r="B162" t="s">
+        <v>105</v>
+      </c>
+      <c r="C162" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B163" t="s">
         <v>107</v>
       </c>
-      <c r="C162" s="7" t="s">
+      <c r="C163" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B163" s="9" t="s">
+    <row r="164" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B164" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C163" s="10" t="s">
+      <c r="C164" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2954,25 +2968,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0d55314f-45f1-40c9-9fce-63556e193d03">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F74FB0E003A88C4B9D9793633BA4B356" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="47be61afb57dbdcdac73424092eefa1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d55314f-45f1-40c9-9fce-63556e193d03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e59f5c7e704c6a619606efe0cdd9ac5" ns2:_="">
     <xsd:import namespace="0d55314f-45f1-40c9-9fce-63556e193d03"/>
@@ -3162,10 +3157,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0d55314f-45f1-40c9-9fce-63556e193d03">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC59A38-DB2E-4FA2-8576-7C42CC1FB709}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BA6EBC9-2836-4C62-BDA5-D123B5DD0A68}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0d55314f-45f1-40c9-9fce-63556e193d03"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3181,19 +3205,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BA6EBC9-2836-4C62-BDA5-D123B5DD0A68}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC59A38-DB2E-4FA2-8576-7C42CC1FB709}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0d55314f-45f1-40c9-9fce-63556e193d03"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>